<commit_message>
adjust day 0 calculations to reflect discussion; add aggregated data file
</commit_message>
<xml_diff>
--- a/data/clean/Mini Trial FS FIB TS&VS_nick.xlsx
+++ b/data/clean/Mini Trial FS FIB TS&VS_nick.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/GitHub/SN_minitrials/data/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F386DFC3-C7DB-4346-BD1A-D0B6930CAA82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165DD7FC-6440-4D44-A791-8B9E0DA12208}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="87">
   <si>
     <t>Crucible weights</t>
   </si>
@@ -259,12 +259,6 @@
     <t># data aggregated from previous sheet</t>
   </si>
   <si>
-    <t># Note that all by TS and VS are repeated values because those were prepared according to the different OL's based on VS</t>
-  </si>
-  <si>
-    <t>TS?</t>
-  </si>
-  <si>
     <t>Ecoli</t>
   </si>
   <si>
@@ -278,6 +272,27 @@
   </si>
   <si>
     <t>per gram</t>
+  </si>
+  <si>
+    <t>coliforms</t>
+  </si>
+  <si>
+    <t>coli</t>
+  </si>
+  <si>
+    <t>enterococci</t>
+  </si>
+  <si>
+    <t># Note that all by  VS are repeated values because those were prepared according to the different OL's based on VS</t>
+  </si>
+  <si>
+    <t>nh3</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t># Dummy values of 37 degrees and a pH of 7.97 were added temporairrly, as were the Nas for COD until we get the innoculum values</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU88"/>
+  <dimension ref="A1:AQ88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:Q6"/>
+    <sheetView topLeftCell="K3" zoomScale="99" workbookViewId="0">
+      <selection activeCell="AC23" sqref="AC23:AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,9 +1100,10 @@
     <col min="17" max="17" width="12.83203125" customWidth="1"/>
     <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.33203125" customWidth="1"/>
+    <col min="36" max="38" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="48"/>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -1103,11 +1119,8 @@
       <c r="M1" s="48"/>
       <c r="N1" s="48"/>
       <c r="O1" s="48"/>
-      <c r="AJ1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>14</v>
       </c>
@@ -1138,19 +1151,10 @@
         <v>61</v>
       </c>
       <c r="AJ2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AS2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1243,6 +1247,9 @@
       <c r="AG3" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="AI3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="AJ3" s="1" t="s">
         <v>57</v>
       </c>
@@ -1252,35 +1259,8 @@
       <c r="AL3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AM3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1365,11 +1345,11 @@
         <v>36.447805461673404</v>
       </c>
       <c r="Z4" s="9">
-        <f t="shared" ref="Z4:AA4" si="0">36+W4</f>
+        <f t="shared" ref="Z4" si="0">36+W4</f>
         <v>37.79122184669361</v>
       </c>
       <c r="AA4" s="9">
-        <f t="shared" si="0"/>
+        <f>36+X4</f>
         <v>39.134638231713822</v>
       </c>
       <c r="AB4" s="32">
@@ -1396,56 +1376,20 @@
         <f>((O4*X4)+(O14*36))/(X14+X4)</f>
         <v>5.6526788019052514</v>
       </c>
-      <c r="AJ4" s="9">
-        <f>(0.5*7*0.036)*100/N4</f>
-        <v>0.36483860954045061</v>
-      </c>
-      <c r="AK4" s="9">
-        <f>(2*7*0.036)/(N4/100)</f>
-        <v>1.4593544381618027</v>
-      </c>
-      <c r="AL4" s="9">
-        <f>(3.5*7*0.036)*100/N4</f>
-        <v>2.5538702667831541</v>
-      </c>
-      <c r="AM4" s="9">
-        <f>36+AJ4</f>
-        <v>36.364838609540449</v>
-      </c>
-      <c r="AN4" s="9">
-        <f>36+AK4</f>
-        <v>37.459354438161803</v>
-      </c>
-      <c r="AO4" s="9">
-        <f>36+AL4</f>
-        <v>38.553870266783157</v>
-      </c>
-      <c r="AP4" s="32">
-        <f>((N4*AJ4)+(N14*36))/AM4</f>
-        <v>5.8679326232860527</v>
-      </c>
-      <c r="AQ4" s="32">
-        <f>((N4*AK4)+(N14*36))/AN4</f>
-        <v>6.7055726556130368</v>
-      </c>
-      <c r="AR4" s="32">
-        <f>((N4*AL4)+(N14*36))/AO4</f>
-        <v>7.4956527274107811</v>
-      </c>
-      <c r="AS4" s="32">
-        <f>(($N4*AJ4)+($N14*36))/(V14+AJ4)</f>
-        <v>5.9410926826545722</v>
-      </c>
-      <c r="AT4" s="32">
-        <f>(($N4*AK4)+($N14*36))/(W14+AK4)</f>
-        <v>7.0423205412648473</v>
-      </c>
-      <c r="AU4" s="32">
-        <f t="shared" ref="AU4" si="1">(($N4*AL4)+($N14*36))/(X14+AL4)</f>
-        <v>8.1590256539532806</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ4" s="32">
+        <f>(($N4*V4)+($N14*36))/(V14+V4)</f>
+        <v>6.006993082334283</v>
+      </c>
+      <c r="AK4" s="32">
+        <f>(($N4*W4)+($N14*36))/(W14+W4)</f>
+        <v>7.2957704278825792</v>
+      </c>
+      <c r="AL4" s="32">
+        <f>(($N4*X4)+($N14*36))/(X14+X4)</f>
+        <v>8.5845477734308773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1400,7 @@
         <v>29.520499999999998</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D12" si="2">C5-B5</f>
+        <f t="shared" ref="D5:D12" si="1">C5-B5</f>
         <v>9.1979999999999968</v>
       </c>
       <c r="E5" s="2">
@@ -1467,24 +1411,24 @@
         <v>20.917899999999999</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H12" si="3">E5-B5</f>
+        <f t="shared" ref="H5:H12" si="2">E5-B5</f>
         <v>3.1745999999999981</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I12" si="4">E5-G5</f>
+        <f t="shared" ref="I5:I12" si="3">E5-G5</f>
         <v>2.5792000000000002</v>
       </c>
       <c r="J5" s="47"/>
       <c r="K5" s="2">
-        <f t="shared" ref="K5:K8" si="5">(H5/D5)*100</f>
+        <f t="shared" ref="K5:K8" si="4">(H5/D5)*100</f>
         <v>34.514024787997386</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L12" si="6">(I5/D5)*100</f>
+        <f t="shared" ref="L5:L12" si="5">(I5/D5)*100</f>
         <v>28.040878451837369</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M12" si="7">I5/H5*100</f>
+        <f t="shared" ref="M5:M12" si="6">I5/H5*100</f>
         <v>81.244881244881299</v>
       </c>
       <c r="N5" s="47"/>
@@ -1509,17 +1453,8 @@
       <c r="AJ5" s="9"/>
       <c r="AK5" s="9"/>
       <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="9"/>
-      <c r="AU5" s="9"/>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1530,7 +1465,7 @@
         <v>27.630199999999999</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.2600999999999978</v>
       </c>
       <c r="E6" s="2">
@@ -1541,24 +1476,24 @@
         <v>20.8185</v>
       </c>
       <c r="H6" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5092999999999996</v>
+      </c>
+      <c r="I6" s="2">
         <f t="shared" si="3"/>
-        <v>2.5092999999999996</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="4"/>
         <v>2.0609000000000002</v>
       </c>
       <c r="J6" s="47"/>
       <c r="K6" s="2">
+        <f t="shared" si="4"/>
+        <v>34.562884808749196</v>
+      </c>
+      <c r="L6" s="2">
         <f t="shared" si="5"/>
-        <v>34.562884808749196</v>
-      </c>
-      <c r="L6" s="2">
+        <v>28.386661340752894</v>
+      </c>
+      <c r="M6" s="2">
         <f t="shared" si="6"/>
-        <v>28.386661340752894</v>
-      </c>
-      <c r="M6" s="2">
-        <f t="shared" si="7"/>
         <v>82.130474634360198</v>
       </c>
       <c r="N6" s="47"/>
@@ -1583,17 +1518,8 @@
       <c r="AJ6" s="9"/>
       <c r="AK6" s="9"/>
       <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-      <c r="AU6" s="9"/>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1604,7 +1530,7 @@
         <v>42.941499999999998</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22.546599999999998</v>
       </c>
       <c r="E7" s="2">
@@ -1618,11 +1544,11 @@
         <v>20.799600000000002</v>
       </c>
       <c r="H7" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8694999999999986</v>
+      </c>
+      <c r="I7" s="2">
         <f t="shared" si="3"/>
-        <v>1.8694999999999986</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="4"/>
         <v>1.4647999999999968</v>
       </c>
       <c r="J7" s="47">
@@ -1630,15 +1556,15 @@
         <v>1.3685333333333329</v>
       </c>
       <c r="K7" s="2">
+        <f t="shared" si="4"/>
+        <v>8.2917158241153821</v>
+      </c>
+      <c r="L7" s="2">
         <f t="shared" si="5"/>
-        <v>8.2917158241153821</v>
-      </c>
-      <c r="L7" s="2">
+        <v>6.4967666965307274</v>
+      </c>
+      <c r="M7" s="2">
         <f t="shared" si="6"/>
-        <v>6.4967666965307274</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="7"/>
         <v>78.352500668627854</v>
       </c>
       <c r="N7" s="47">
@@ -1658,7 +1584,7 @@
         <v>19</v>
       </c>
       <c r="T7" s="45">
-        <f t="shared" ref="T7" si="8">S7*100</f>
+        <f t="shared" ref="T7" si="7">S7*100</f>
         <v>1900</v>
       </c>
       <c r="V7" s="9">
@@ -1678,11 +1604,11 @@
         <v>37.941215106823172</v>
       </c>
       <c r="Z7" s="9">
-        <f t="shared" ref="Z7:AA7" si="9">36+W7</f>
+        <f t="shared" ref="Z7:AA7" si="8">36+W7</f>
         <v>43.764860427292682</v>
       </c>
       <c r="AA7" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>49.588505747762191</v>
       </c>
       <c r="AB7" s="32">
@@ -1709,56 +1635,20 @@
         <f>((O7*X7)+(O14*36))/(X15+X7)</f>
         <v>5.6526788019052514</v>
       </c>
-      <c r="AJ7" s="9">
-        <f>(0.5*7*0.036)*100/N7</f>
-        <v>1.5209752940650267</v>
-      </c>
-      <c r="AK7" s="9">
-        <f>(2*7*0.036)/(N7/100)</f>
-        <v>6.083901176260107</v>
-      </c>
-      <c r="AL7" s="9">
-        <f>(3.5*7*0.036)*100/N7</f>
-        <v>10.646827058455186</v>
-      </c>
-      <c r="AM7" s="9">
-        <f>36+AJ7</f>
-        <v>37.520975294065025</v>
-      </c>
-      <c r="AN7" s="9">
-        <f t="shared" ref="AN7" si="10">36+AK7</f>
-        <v>42.083901176260106</v>
-      </c>
-      <c r="AO7" s="9">
-        <f t="shared" ref="AO7" si="11">36+AL7</f>
-        <v>46.646827058455187</v>
-      </c>
-      <c r="AP7" s="32">
-        <f>((N7*AJ7)+(N14*36))/AM7</f>
-        <v>5.6871235660872479</v>
-      </c>
-      <c r="AQ7" s="32">
-        <f>((N7*AK7)+(N14*36))/AN7</f>
-        <v>5.9687057472502349</v>
-      </c>
-      <c r="AR7" s="32">
-        <f>((N7*AL7)+(N14*36))/AO7</f>
-        <v>6.1951999962465401</v>
-      </c>
-      <c r="AS7" s="32">
-        <f>(($N7*AJ7)+($N14*36))/(V15+AJ7)</f>
-        <v>5.9974103730460344</v>
-      </c>
-      <c r="AT7" s="32">
-        <f t="shared" ref="AT7" si="12">(($N7*AK7)+($N14*36))/(W15+AK7)</f>
-        <v>7.3191562857132659</v>
-      </c>
-      <c r="AU7" s="32">
-        <f>(($N7*AL7)+($N14*36))/(X15+AL7)</f>
-        <v>8.7417149861139336</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ7" s="32">
+        <f>(($N7*V7)+($N14*36))/(V15+V7)</f>
+        <v>6.0241043311361375</v>
+      </c>
+      <c r="AK7" s="32">
+        <f t="shared" ref="AK7:AL7" si="9">(($N7*W7)+($N14*36))/(W15+W7)</f>
+        <v>7.3642154230899983</v>
+      </c>
+      <c r="AL7" s="32">
+        <f t="shared" si="9"/>
+        <v>8.7043265150438618</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1769,7 +1659,7 @@
         <v>40.8337</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20.501999999999999</v>
       </c>
       <c r="E8" s="2">
@@ -1784,20 +1674,20 @@
         <v>1.7012999999999998</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.3362000000000016</v>
       </c>
       <c r="J8" s="47"/>
       <c r="K8" s="2">
+        <f t="shared" si="4"/>
+        <v>8.2982148083113838</v>
+      </c>
+      <c r="L8" s="2">
         <f t="shared" si="5"/>
-        <v>8.2982148083113838</v>
-      </c>
-      <c r="L8" s="2">
+        <v>6.5174129353233914</v>
+      </c>
+      <c r="M8" s="2">
         <f t="shared" si="6"/>
-        <v>6.5174129353233914</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="7"/>
         <v>78.539940045847402</v>
       </c>
       <c r="N8" s="47"/>
@@ -1822,17 +1712,8 @@
       <c r="AJ8" s="9"/>
       <c r="AK8" s="9"/>
       <c r="AL8" s="9"/>
-      <c r="AM8" s="9"/>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="9"/>
-      <c r="AP8" s="9"/>
-      <c r="AQ8" s="9"/>
-      <c r="AR8" s="9"/>
-      <c r="AS8" s="9"/>
-      <c r="AT8" s="9"/>
-      <c r="AU8" s="9"/>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1843,7 +1724,7 @@
         <v>40.435099999999998</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20.200799999999997</v>
       </c>
       <c r="E9" s="2">
@@ -1854,11 +1735,11 @@
         <v>20.598800000000001</v>
       </c>
       <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6691000000000003</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="3"/>
-        <v>1.6691000000000003</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="4"/>
         <v>1.3046000000000006</v>
       </c>
       <c r="J9" s="47"/>
@@ -1867,11 +1748,11 @@
         <v>8.2625440576610849</v>
       </c>
       <c r="L9" s="2">
+        <f t="shared" si="5"/>
+        <v>6.458160072868405</v>
+      </c>
+      <c r="M9" s="2">
         <f t="shared" si="6"/>
-        <v>6.458160072868405</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="7"/>
         <v>78.161883649871214</v>
       </c>
       <c r="N9" s="47"/>
@@ -1896,17 +1777,8 @@
       <c r="AJ9" s="9"/>
       <c r="AK9" s="9"/>
       <c r="AL9" s="9"/>
-      <c r="AM9" s="9"/>
-      <c r="AN9" s="9"/>
-      <c r="AO9" s="9"/>
-      <c r="AP9" s="9"/>
-      <c r="AQ9" s="9"/>
-      <c r="AR9" s="9"/>
-      <c r="AS9" s="9"/>
-      <c r="AT9" s="9"/>
-      <c r="AU9" s="9"/>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1917,7 +1789,7 @@
         <v>36.075899999999997</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15.369499999999999</v>
       </c>
       <c r="E10" s="2">
@@ -1931,11 +1803,11 @@
         <v>21.194500000000001</v>
       </c>
       <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5143000000000022</v>
+      </c>
+      <c r="I10" s="2">
         <f t="shared" si="3"/>
-        <v>2.5143000000000022</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="4"/>
         <v>2.0261999999999993</v>
       </c>
       <c r="J10" s="47">
@@ -1947,11 +1819,11 @@
         <v>16.359022739841912</v>
       </c>
       <c r="L10" s="2">
+        <f t="shared" si="5"/>
+        <v>13.183252545626075</v>
+      </c>
+      <c r="M10" s="2">
         <f t="shared" si="6"/>
-        <v>13.183252545626075</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="7"/>
         <v>80.587042119078774</v>
       </c>
       <c r="N10" s="47">
@@ -1971,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="T10" s="45">
-        <f t="shared" ref="T10" si="13">S10*100</f>
+        <f t="shared" ref="T10" si="10">S10*100</f>
         <v>1200</v>
       </c>
       <c r="V10" s="9">
@@ -1991,11 +1863,11 @@
         <v>36.951410350188574</v>
       </c>
       <c r="Z10" s="9">
-        <f t="shared" ref="Z10:AA10" si="14">36+W10</f>
+        <f t="shared" ref="Z10:AA10" si="11">36+W10</f>
         <v>39.805641400754311</v>
       </c>
       <c r="AA10" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>42.659872451320041</v>
       </c>
       <c r="AB10" s="32">
@@ -2022,56 +1894,20 @@
         <f>((O10*X10)+(O14*36))/(X16+X10)</f>
         <v>5.6526788019052514</v>
       </c>
-      <c r="AJ10" s="9">
-        <f>(0.5*7*0.036)*100/N10</f>
-        <v>0.76732316110454668</v>
-      </c>
-      <c r="AK10" s="9">
-        <f>(2*7*0.036)/(N10/100)</f>
-        <v>3.0692926444181867</v>
-      </c>
-      <c r="AL10" s="9">
-        <f>(3.5*7*0.036)*100/N10</f>
-        <v>5.3712621277318258</v>
-      </c>
-      <c r="AM10" s="9">
-        <f>36+AJ10</f>
-        <v>36.767323161104549</v>
-      </c>
-      <c r="AN10" s="9">
-        <f t="shared" ref="AN10" si="15">36+AK10</f>
-        <v>39.069292644418184</v>
-      </c>
-      <c r="AO10" s="9">
-        <f t="shared" ref="AO10" si="16">36+AL10</f>
-        <v>41.371262127731825</v>
-      </c>
-      <c r="AP10" s="32">
-        <f>((N10*AJ10)+(N14*36))/AM10</f>
-        <v>5.8036975355114251</v>
-      </c>
-      <c r="AQ10" s="32">
-        <f>((N10*AK10)+(N14*36))/AN10</f>
-        <v>6.429254430162854</v>
-      </c>
-      <c r="AR10" s="32">
-        <f>((N10*AL10)+(N14*36))/AO10</f>
-        <v>6.9851971623496185</v>
-      </c>
-      <c r="AS10" s="32">
-        <f>(($N10*AJ10)+($N14*36))/(V16+AJ10)</f>
-        <v>5.9578663803430603</v>
-      </c>
-      <c r="AT10" s="32">
-        <f t="shared" ref="AT10:AU10" si="17">(($N10*AK10)+($N14*36))/(W16+AK10)</f>
-        <v>7.1230974093355544</v>
-      </c>
-      <c r="AU10" s="32">
-        <f t="shared" si="17"/>
-        <v>8.3254063150872923</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ10" s="32">
+        <f>(($N10*V10)+($N14*36))/(V16+V10)</f>
+        <v>6.011368536059873</v>
+      </c>
+      <c r="AK10" s="32">
+        <f t="shared" ref="AK10" si="12">(($N10*W10)+($N14*36))/(W16+W10)</f>
+        <v>7.313272242784941</v>
+      </c>
+      <c r="AL10" s="32">
+        <f>(($N10*X10)+($N14*36))/(X16+X10)</f>
+        <v>8.6151759495100091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2082,7 +1918,7 @@
         <v>35.125100000000003</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.793900000000004</v>
       </c>
       <c r="E11" s="2">
@@ -2093,11 +1929,11 @@
         <v>20.8371</v>
       </c>
       <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>2.4253</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="3"/>
-        <v>2.4253</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="4"/>
         <v>1.9193999999999996</v>
       </c>
       <c r="J11" s="47"/>
@@ -2106,11 +1942,11 @@
         <v>16.393919115311036</v>
       </c>
       <c r="L11" s="2">
+        <f t="shared" si="5"/>
+        <v>12.974266420619301</v>
+      </c>
+      <c r="M11" s="2">
         <f t="shared" si="6"/>
-        <v>12.974266420619301</v>
-      </c>
-      <c r="M11" s="2">
-        <f t="shared" si="7"/>
         <v>79.140724858780345</v>
       </c>
       <c r="N11" s="47"/>
@@ -2121,7 +1957,7 @@
       <c r="S11" s="45"/>
       <c r="T11" s="45"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2132,7 +1968,7 @@
         <v>35.959600000000002</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15.645800000000001</v>
       </c>
       <c r="E12" s="2">
@@ -2143,11 +1979,11 @@
         <v>20.773199999999999</v>
       </c>
       <c r="H12" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5829999999999984</v>
+      </c>
+      <c r="I12" s="2">
         <f t="shared" si="3"/>
-        <v>2.5829999999999984</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="4"/>
         <v>2.1235999999999997</v>
       </c>
       <c r="J12" s="47"/>
@@ -2156,11 +1992,11 @@
         <v>16.50922292244563</v>
       </c>
       <c r="L12" s="2">
+        <f t="shared" si="5"/>
+        <v>13.572971660126038</v>
+      </c>
+      <c r="M12" s="2">
         <f t="shared" si="6"/>
-        <v>13.572971660126038</v>
-      </c>
-      <c r="M12" s="2">
-        <f t="shared" si="7"/>
         <v>82.21447928765005</v>
       </c>
       <c r="N12" s="47"/>
@@ -2171,7 +2007,7 @@
       <c r="S12" s="45"/>
       <c r="T12" s="45"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2191,10 +2027,10 @@
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
       <c r="V13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2219,11 +2055,11 @@
         <v>21.099699999999999</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" ref="H14:H16" si="18">E14-B14</f>
+        <f t="shared" ref="H14:H16" si="13">E14-B14</f>
         <v>1.3828999999999994</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" ref="I14:I16" si="19">E14-G14</f>
+        <f t="shared" ref="I14:I16" si="14">E14-G14</f>
         <v>0.801400000000001</v>
       </c>
       <c r="J14" s="47">
@@ -2235,11 +2071,11 @@
         <v>5.5686201870031953</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" ref="L14:L16" si="20">(I14/D14)*100</f>
+        <f t="shared" ref="L14:L16" si="15">(I14/D14)*100</f>
         <v>3.2270534513445428</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" ref="M14:M16" si="21">I14/H14*100</f>
+        <f t="shared" ref="M14:M16" si="16">I14/H14*100</f>
         <v>57.950683346590594</v>
       </c>
       <c r="N14" s="47">
@@ -2259,7 +2095,7 @@
         <v>20</v>
       </c>
       <c r="T14" s="45">
-        <f t="shared" ref="T14" si="22">S14*100</f>
+        <f t="shared" ref="T14" si="17">S14*100</f>
         <v>2000</v>
       </c>
       <c r="U14" t="s">
@@ -2270,15 +2106,15 @@
         <v>35.552194538326596</v>
       </c>
       <c r="W14" s="9">
-        <f t="shared" ref="W14:X14" si="23">SUM(36-W4)</f>
+        <f t="shared" ref="W14:X14" si="18">SUM(36-W4)</f>
         <v>34.20877815330639</v>
       </c>
       <c r="X14" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>32.865361768286178</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2289,7 +2125,7 @@
         <v>46.766300000000001</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:D16" si="24">C15-B15</f>
+        <f t="shared" ref="D15:D16" si="19">C15-B15</f>
         <v>26.016200000000001</v>
       </c>
       <c r="E15" s="2">
@@ -2300,11 +2136,11 @@
         <v>21.369299999999999</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>1.4494000000000007</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.83020000000000138</v>
       </c>
       <c r="J15" s="47"/>
@@ -2313,11 +2149,11 @@
         <v>5.5711441332708107</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>3.1910886293924605</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>57.278874016834621</v>
       </c>
       <c r="N15" s="47"/>
@@ -2335,15 +2171,18 @@
         <v>34.058784893176828</v>
       </c>
       <c r="W15" s="9">
-        <f t="shared" ref="W15:X15" si="25">SUM(36-W7)</f>
+        <f t="shared" ref="W15:X15" si="20">SUM(36-W7)</f>
         <v>28.235139572707318</v>
       </c>
       <c r="X15" s="9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>22.411494252237809</v>
       </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2354,7 +2193,7 @@
         <v>45.366399999999999</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>24.944399999999998</v>
       </c>
       <c r="E16" s="2">
@@ -2365,11 +2204,11 @@
         <v>21.0213</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>1.3949999999999996</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0.79570000000000007</v>
       </c>
       <c r="J16" s="47"/>
@@ -2378,11 +2217,11 @@
         <v>5.592437581180544</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>3.189894324978753</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>57.039426523297507</v>
       </c>
       <c r="N16" s="47"/>
@@ -2400,15 +2239,27 @@
         <v>35.048589649811426</v>
       </c>
       <c r="W16" s="9">
-        <f t="shared" ref="W16:X16" si="26">SUM(36-W10)</f>
+        <f t="shared" ref="W16:X16" si="21">SUM(36-W10)</f>
         <v>32.194358599245689</v>
       </c>
       <c r="X16" s="9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>29.340127548679963</v>
       </c>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AI16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2424,14 +2275,29 @@
       <c r="R17" s="11"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ17" s="32">
+        <f>(($I23*V4)+($I28*36))/(V14+V4)</f>
+        <v>1977.9080842054786</v>
+      </c>
+      <c r="AK17" s="32">
+        <f>(($N17*W17)+($N27*36))/(W27+W17)</f>
+        <v>0</v>
+      </c>
+      <c r="AL17" s="32">
+        <f>(($N17*X17)+($N27*36))/(X27+X17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="7"/>
       <c r="C18" s="2"/>
       <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="9"/>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>40</v>
       </c>
@@ -2459,8 +2325,11 @@
       <c r="I19" s="21"/>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="25"/>
       <c r="B20" s="22" t="s">
         <v>32</v>
@@ -2489,8 +2358,20 @@
       <c r="I20" s="22"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
-    </row>
-    <row r="21" spans="1:47" ht="34" x14ac:dyDescent="0.2">
+      <c r="AJ20" s="32" t="e">
+        <f>(($N20*V20)+($N27*36))/(V28+V20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK20" s="32" t="e">
+        <f t="shared" ref="AK20" si="22">(($N20*W20)+($N27*36))/(W28+W20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL20" s="32" t="e">
+        <f t="shared" ref="AL20" si="23">(($N20*X20)+($N27*36))/(X28+X20)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="29"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25" t="s">
@@ -2540,10 +2421,11 @@
       <c r="AE21" s="27"/>
       <c r="AF21" s="22"/>
       <c r="AG21" s="32"/>
-      <c r="AS21" s="32"/>
-      <c r="AU21" s="32"/>
-    </row>
-    <row r="22" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
+    </row>
+    <row r="22" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>41</v>
       </c>
@@ -2585,11 +2467,13 @@
       <c r="R22" s="37"/>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
-      <c r="U22" s="39"/>
+      <c r="U22" s="39" t="s">
+        <v>84</v>
+      </c>
       <c r="V22" s="33"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="32"/>
+      <c r="W22" t="s">
+        <v>61</v>
+      </c>
       <c r="Z22" s="32"/>
       <c r="AA22" s="26"/>
       <c r="AB22" s="34"/>
@@ -2598,10 +2482,11 @@
       <c r="AE22" s="37"/>
       <c r="AF22" s="38"/>
       <c r="AG22" s="39"/>
-      <c r="AS22" s="9"/>
-      <c r="AU22" s="32"/>
-    </row>
-    <row r="23" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
+      <c r="AL22" s="9"/>
+    </row>
+    <row r="23" spans="1:43" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="21" t="s">
         <v>42</v>
@@ -2610,22 +2495,22 @@
         <v>3.95</v>
       </c>
       <c r="D23" s="26">
-        <f t="shared" ref="D23:D30" si="27">$D$20</f>
+        <f t="shared" ref="D23:D30" si="24">$D$20</f>
         <v>4.7149999999999999</v>
       </c>
       <c r="E23" s="34">
-        <f t="shared" ref="E23:E30" si="28">$H$20</f>
+        <f t="shared" ref="E23:E30" si="25">$H$20</f>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F23" s="35">
-        <f t="shared" ref="F23:F30" si="29">(D23-C23)*E23*4000</f>
+        <f t="shared" ref="F23:F30" si="26">(D23-C23)*E23*4000</f>
         <v>82.655394321766508</v>
       </c>
       <c r="G23" s="36">
         <v>1000</v>
       </c>
       <c r="H23" s="37">
-        <f t="shared" ref="H23:H30" si="30">F23*G23</f>
+        <f t="shared" ref="H23:H30" si="27">F23*G23</f>
         <v>82655.394321766507</v>
       </c>
       <c r="I23" s="40">
@@ -2648,21 +2533,43 @@
       <c r="T23" s="38"/>
       <c r="U23" s="38"/>
       <c r="V23" s="33"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
+      <c r="W23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="Z23" s="32"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="34"/>
-      <c r="AC23" s="35"/>
+      <c r="AA23" s="26">
+        <v>2004.6024450227544</v>
+      </c>
+      <c r="AB23" s="34">
+        <v>2018.4097800910176</v>
+      </c>
+      <c r="AC23" s="35">
+        <v>2032.2171151592811</v>
+      </c>
       <c r="AD23" s="36"/>
       <c r="AE23" s="37"/>
       <c r="AF23" s="38"/>
       <c r="AG23" s="38"/>
-      <c r="AS23" s="9"/>
-      <c r="AU23" s="32"/>
-    </row>
-    <row r="24" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ23" s="32" t="e">
+        <f>(($N23*V23)+($N27*36))/(V29+V23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK23" s="32" t="e">
+        <f t="shared" ref="AK23" si="28">(($N23*W23)+($N27*36))/(W29+W23)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL23" s="32" t="e">
+        <f>(($N23*X23)+($N27*36))/(X29+X23)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
       <c r="B24" s="21" t="s">
         <v>42</v>
@@ -2671,22 +2578,22 @@
         <v>3.96</v>
       </c>
       <c r="D24" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E24" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F24" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>81.574931650893774</v>
       </c>
       <c r="G24" s="36">
         <v>1000</v>
       </c>
       <c r="H24" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>81574.931650893777</v>
       </c>
       <c r="I24" s="38" t="s">
@@ -2704,18 +2611,35 @@
       <c r="T24" s="41"/>
       <c r="U24" s="41"/>
       <c r="V24" s="41"/>
-      <c r="W24" s="21"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="35"/>
+      <c r="W24" s="32">
+        <f>(($T4*V4)+($T14*36))/(V14+V4)</f>
+        <v>2004.6024450227544</v>
+      </c>
+      <c r="X24" s="32">
+        <f t="shared" ref="X24:Y24" si="29">(($T4*W4)+($T14*36))/(W14+W4)</f>
+        <v>2018.4097800910176</v>
+      </c>
+      <c r="Y24" s="32">
+        <f t="shared" si="29"/>
+        <v>2032.2171151592811</v>
+      </c>
+      <c r="AA24">
+        <v>2102.4530195267785</v>
+      </c>
+      <c r="AB24">
+        <v>2409.8120781071138</v>
+      </c>
+      <c r="AC24">
+        <v>2717.1711366874492</v>
+      </c>
       <c r="AD24" s="36"/>
       <c r="AE24" s="37"/>
       <c r="AF24" s="38"/>
       <c r="AG24" s="38"/>
-      <c r="AS24" s="32"/>
-      <c r="AU24" s="32"/>
-    </row>
-    <row r="25" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ24" s="32"/>
+      <c r="AL24" s="32"/>
+    </row>
+    <row r="25" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
         <v>43</v>
       </c>
@@ -2723,22 +2647,22 @@
         <v>2.95</v>
       </c>
       <c r="D25" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E25" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F25" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>190.70166140904306</v>
       </c>
       <c r="G25" s="36">
         <v>1000</v>
       </c>
       <c r="H25" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>190701.66140904307</v>
       </c>
       <c r="I25" s="40">
@@ -2761,10 +2685,22 @@
       <c r="T25" s="33"/>
       <c r="U25" s="33"/>
       <c r="V25" s="33"/>
-      <c r="AS25" s="9"/>
-      <c r="AU25" s="9"/>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="AA25">
+        <v>2031.713678339619</v>
+      </c>
+      <c r="AB25">
+        <v>2126.8547133584771</v>
+      </c>
+      <c r="AC25">
+        <v>2221.9957483773346</v>
+      </c>
+      <c r="AJ25" s="9"/>
+      <c r="AL25" s="9"/>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26" s="33"/>
       <c r="B26" s="21" t="s">
         <v>43</v>
@@ -2773,22 +2709,22 @@
         <v>2.17</v>
       </c>
       <c r="D26" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E26" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F26" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>274.97774973711876</v>
       </c>
       <c r="G26" s="36">
         <v>1000</v>
       </c>
       <c r="H26" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>274977.74973711878</v>
       </c>
       <c r="I26" s="38"/>
@@ -2805,10 +2741,13 @@
       <c r="T26" s="33"/>
       <c r="U26" s="33"/>
       <c r="V26" s="33"/>
-      <c r="AS26" s="9"/>
-      <c r="AU26" s="9"/>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="AJ26" s="9"/>
+      <c r="AL26" s="9"/>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27" s="33"/>
       <c r="B27" s="21" t="s">
         <v>43</v>
@@ -2817,22 +2756,22 @@
         <v>3.26</v>
       </c>
       <c r="D27" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E27" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F27" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>157.20731861198738</v>
       </c>
       <c r="G27" s="36">
         <v>1000</v>
       </c>
       <c r="H27" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>157207.31861198737</v>
       </c>
       <c r="I27" s="38"/>
@@ -2849,10 +2788,23 @@
       <c r="T27" s="41"/>
       <c r="U27" s="41"/>
       <c r="V27" s="41"/>
-      <c r="AS27" s="32"/>
-      <c r="AU27" s="32"/>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="W27" s="32">
+        <f>(($T7*V7)+($T14*36))/(V15+V7)</f>
+        <v>2102.4530195267785</v>
+      </c>
+      <c r="X27" s="32">
+        <f t="shared" ref="X27:Y27" si="30">(($T7*W7)+($T14*36))/(W15+W7)</f>
+        <v>2409.8120781071138</v>
+      </c>
+      <c r="Y27" s="32">
+        <f t="shared" si="30"/>
+        <v>2717.1711366874492</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="21" t="s">
         <v>44</v>
       </c>
@@ -2860,22 +2812,22 @@
         <v>3.07</v>
       </c>
       <c r="D28" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E28" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F28" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>177.73610935856991</v>
       </c>
       <c r="G28" s="36">
         <v>1000</v>
       </c>
       <c r="H28" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>177736.1093585699</v>
       </c>
       <c r="I28" s="38"/>
@@ -2892,8 +2844,35 @@
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="V28" s="41"/>
-    </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="AI28" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN28" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29" s="33"/>
       <c r="B29" s="21" t="s">
         <v>44</v>
@@ -2902,22 +2881,22 @@
         <v>3.27</v>
       </c>
       <c r="D29" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E29" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F29" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>156.12685594111457</v>
       </c>
       <c r="G29" s="36">
         <v>1000</v>
       </c>
       <c r="H29" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>156126.85594111457</v>
       </c>
       <c r="I29" s="38"/>
@@ -2934,8 +2913,35 @@
       <c r="T29" s="33"/>
       <c r="U29" s="33"/>
       <c r="V29" s="33"/>
-    </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="AJ29" s="32">
+        <f>(($C73*$V4)+($C76*36))/($V14+$V4)</f>
+        <v>49931.772002135534</v>
+      </c>
+      <c r="AK29" s="32">
+        <f>(($C73*$W4)+($C76*36))/($W14+$W4)</f>
+        <v>198827.08800854211</v>
+      </c>
+      <c r="AL29" s="32">
+        <f>(($C73*$X4)+($C76*36))/($X14+$X4)</f>
+        <v>347722.40401494864</v>
+      </c>
+      <c r="AN29">
+        <v>2</v>
+      </c>
+      <c r="AO29">
+        <v>49931.772002135534</v>
+      </c>
+      <c r="AP29">
+        <v>198827.08800854211</v>
+      </c>
+      <c r="AQ29">
+        <v>347722.40401494864</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="21" t="s">
         <v>44</v>
@@ -2944,29 +2950,56 @@
         <v>2.76</v>
       </c>
       <c r="D30" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E30" s="34">
-        <f t="shared" si="28"/>
+        <f t="shared" si="25"/>
         <v>2.7011566771819134E-2</v>
       </c>
       <c r="F30" s="35">
-        <f t="shared" si="29"/>
+        <f t="shared" si="26"/>
         <v>211.23045215562564</v>
       </c>
       <c r="G30" s="36">
         <v>1000</v>
       </c>
       <c r="H30" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>211230.45215562565</v>
       </c>
       <c r="T30" s="33"/>
       <c r="U30" s="33"/>
       <c r="V30" s="33"/>
-    </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="W30" s="32">
+        <f>(($T10*V10)+($T14*36))/(V16+V10)</f>
+        <v>2031.713678339619</v>
+      </c>
+      <c r="X30" s="32">
+        <f t="shared" ref="X30:Y30" si="31">(($T10*W10)+($T14*36))/(W16+W10)</f>
+        <v>2126.8547133584771</v>
+      </c>
+      <c r="Y30" s="32">
+        <f t="shared" si="31"/>
+        <v>2221.9957483773346</v>
+      </c>
+      <c r="AJ30" s="9"/>
+      <c r="AK30" s="9"/>
+      <c r="AL30" s="9"/>
+      <c r="AN30">
+        <v>3</v>
+      </c>
+      <c r="AO30">
+        <v>469642.67471635767</v>
+      </c>
+      <c r="AP30">
+        <v>1877670.6988654307</v>
+      </c>
+      <c r="AQ30">
+        <v>3285698.7230145033</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="21"/>
       <c r="D31" s="26"/>
@@ -2974,8 +3007,23 @@
       <c r="T31" s="41"/>
       <c r="U31" s="41"/>
       <c r="V31" s="41"/>
-    </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="9"/>
+      <c r="AL31" s="9"/>
+      <c r="AN31">
+        <v>4</v>
+      </c>
+      <c r="AO31">
+        <v>240266.83276978548</v>
+      </c>
+      <c r="AP31">
+        <v>960167.33107914194</v>
+      </c>
+      <c r="AQ31">
+        <v>1680067.8293884983</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>40</v>
       </c>
@@ -3002,8 +3050,32 @@
       </c>
       <c r="I32" s="21"/>
       <c r="J32" s="24"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ32" s="32">
+        <f>(($C74*$V7)+($C76*36))/($V15+$V7)</f>
+        <v>469642.67471635767</v>
+      </c>
+      <c r="AK32" s="32">
+        <f>(($C74*$W7)+($C76*36))/($W15+$W7)</f>
+        <v>1877670.6988654307</v>
+      </c>
+      <c r="AL32" s="32">
+        <f>(($C74*$X7)+($C76*36))/($X15+$X7)</f>
+        <v>3285698.7230145033</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO32">
+        <v>40675.662768667476</v>
+      </c>
+      <c r="AP32">
+        <v>162702.65107466988</v>
+      </c>
+      <c r="AQ32">
+        <v>284729.63938067225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
       <c r="B33" s="22" t="s">
         <v>32</v>
@@ -3031,8 +3103,20 @@
       </c>
       <c r="I33" s="22"/>
       <c r="J33" s="24"/>
-    </row>
-    <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="AJ33" s="9"/>
+      <c r="AK33" s="9"/>
+      <c r="AL33" s="9"/>
+      <c r="AO33">
+        <v>258073.76392376923</v>
+      </c>
+      <c r="AP33">
+        <v>1032295.0556950769</v>
+      </c>
+      <c r="AQ33">
+        <v>1806516.3474663845</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="25"/>
       <c r="C34" s="25" t="s">
@@ -3059,8 +3143,20 @@
       <c r="J34" s="32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ34" s="9"/>
+      <c r="AK34" s="9"/>
+      <c r="AL34" s="9"/>
+      <c r="AO34">
+        <v>202703.26072073291</v>
+      </c>
+      <c r="AP34">
+        <v>810813.04288293165</v>
+      </c>
+      <c r="AQ34">
+        <v>1418922.8250451302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>45</v>
       </c>
@@ -3092,8 +3188,32 @@
       <c r="I35" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ35" s="32">
+        <f>(($C75*$V10)+($C76*36))/($V16+$V10)</f>
+        <v>240266.83276978548</v>
+      </c>
+      <c r="AK35" s="32">
+        <f>(($C75*$W10)+($C76*36))/($W16+$W10)</f>
+        <v>960167.33107914194</v>
+      </c>
+      <c r="AL35" s="32">
+        <f>(($C75*$X10)+($C76*36))/($X16+$X10)</f>
+        <v>1680067.8293884983</v>
+      </c>
+      <c r="AN35" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO35">
+        <v>102160.56248817024</v>
+      </c>
+      <c r="AP35">
+        <v>105642.24995268096</v>
+      </c>
+      <c r="AQ35">
+        <v>109123.93741719166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
       <c r="B36" s="21" t="s">
         <v>46</v>
@@ -3102,22 +3222,22 @@
         <v>2.44</v>
       </c>
       <c r="D36" s="26">
-        <f t="shared" ref="D36:D43" si="31">$D$33</f>
+        <f t="shared" ref="D36:D43" si="32">$D$33</f>
         <v>5.62</v>
       </c>
       <c r="E36" s="34">
-        <f t="shared" ref="E36:E43" si="32">$H$33</f>
+        <f t="shared" ref="E36:E43" si="33">$H$33</f>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F36" s="35">
-        <f t="shared" ref="F36:F43" si="33">(D36-C36)*E36*4000</f>
+        <f t="shared" ref="F36:F43" si="34">(D36-C36)*E36*4000</f>
         <v>293.5771428571428</v>
       </c>
       <c r="G36" s="36">
         <v>100</v>
       </c>
       <c r="H36" s="37">
-        <f t="shared" ref="H36:H43" si="34">F36*G36</f>
+        <f t="shared" ref="H36:H43" si="35">F36*G36</f>
         <v>29357.714285714279</v>
       </c>
       <c r="I36" s="40">
@@ -3130,8 +3250,17 @@
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="8"/>
-    </row>
-    <row r="37" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO36">
+        <v>127335.81828256769</v>
+      </c>
+      <c r="AP36">
+        <v>206343.27313027071</v>
+      </c>
+      <c r="AQ36">
+        <v>285350.7279779737</v>
+      </c>
+    </row>
+    <row r="37" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
       <c r="B37" s="21" t="s">
         <v>46</v>
@@ -3140,29 +3269,38 @@
         <v>2.86</v>
       </c>
       <c r="D37" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E37" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F37" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>254.80280323450134</v>
       </c>
       <c r="G37" s="36">
         <v>100</v>
       </c>
       <c r="H37" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>25480.280323450133</v>
       </c>
       <c r="I37" s="38" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO37">
+        <v>153494.06607165473</v>
+      </c>
+      <c r="AP37">
+        <v>310976.26428661891</v>
+      </c>
+      <c r="AQ37">
+        <v>468458.46250158298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
         <v>47</v>
       </c>
@@ -3170,22 +3308,22 @@
         <v>2.46</v>
       </c>
       <c r="D38" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E38" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F38" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>291.73074573225517</v>
       </c>
       <c r="G38" s="36">
         <v>100</v>
       </c>
       <c r="H38" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>29173.074573225516</v>
       </c>
       <c r="I38" s="40">
@@ -3197,8 +3335,11 @@
         <v>0.65043835894704471</v>
       </c>
       <c r="N38" s="9"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="33"/>
       <c r="B39" s="21" t="s">
         <v>47</v>
@@ -3207,29 +3348,44 @@
         <v>2.65</v>
       </c>
       <c r="D39" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E39" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F39" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>274.18997304582211</v>
       </c>
       <c r="G39" s="36">
         <v>100</v>
       </c>
       <c r="H39" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>27418.997304582212</v>
       </c>
       <c r="I39" s="38"/>
       <c r="J39" s="38"/>
       <c r="N39" s="9"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AI39" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A40" s="33"/>
       <c r="B40" s="21" t="s">
         <v>47</v>
@@ -3238,28 +3394,40 @@
         <v>2.48</v>
       </c>
       <c r="D40" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E40" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F40" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>289.88434860736743</v>
       </c>
       <c r="G40" s="36">
         <v>100</v>
       </c>
       <c r="H40" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28988.434860736743</v>
       </c>
       <c r="I40" s="38"/>
       <c r="J40" s="38"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ40" s="32">
+        <f>(($E73*V4)+($E76*36))/(V14+V4)</f>
+        <v>40675.662768667476</v>
+      </c>
+      <c r="AK40" s="32">
+        <f t="shared" ref="AK40:AL40" si="36">(($E73*W4)+($E76*36))/(W14+W4)</f>
+        <v>162702.65107466988</v>
+      </c>
+      <c r="AL40" s="32">
+        <f t="shared" si="36"/>
+        <v>284729.63938067225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="B41" s="21" t="s">
         <v>48</v>
       </c>
@@ -3267,28 +3435,31 @@
         <v>2.39</v>
       </c>
       <c r="D41" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E41" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F41" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>298.19313566936205</v>
       </c>
       <c r="G41" s="36">
         <v>100</v>
       </c>
       <c r="H41" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>29819.313566936205</v>
       </c>
       <c r="I41" s="38"/>
       <c r="J41" s="39"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ41" s="9"/>
+      <c r="AK41" s="9"/>
+      <c r="AL41" s="9"/>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A42" s="33"/>
       <c r="B42" s="21" t="s">
         <v>48</v>
@@ -3297,28 +3468,31 @@
         <v>2.21</v>
       </c>
       <c r="D42" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E42" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F42" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>314.81070979335129</v>
       </c>
       <c r="G42" s="36">
         <v>100</v>
       </c>
       <c r="H42" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>31481.070979335131</v>
       </c>
       <c r="I42" s="38"/>
       <c r="J42" s="38"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ42" s="9"/>
+      <c r="AK42" s="9"/>
+      <c r="AL42" s="9"/>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="21" t="s">
         <v>48</v>
@@ -3327,32 +3501,47 @@
         <v>2.5</v>
       </c>
       <c r="D43" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>5.62</v>
       </c>
       <c r="E43" s="34">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.3079964061096133E-2</v>
       </c>
       <c r="F43" s="35">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>288.03795148247974</v>
       </c>
       <c r="G43" s="36">
         <v>100</v>
       </c>
       <c r="H43" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28803.795148247973</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ43" s="32">
+        <f>(($E74*V7)+($E76*36))/(V15+V7)</f>
+        <v>258073.76392376923</v>
+      </c>
+      <c r="AK43" s="32">
+        <f t="shared" ref="AK43:AL43" si="37">(($E74*W7)+($E76*36))/(W15+W7)</f>
+        <v>1032295.0556950769</v>
+      </c>
+      <c r="AL43" s="32">
+        <f t="shared" si="37"/>
+        <v>1806516.3474663845</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="21"/>
       <c r="D44" s="26"/>
       <c r="E44" s="34"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ44" s="9"/>
+      <c r="AK44" s="9"/>
+      <c r="AL44" s="9"/>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>40</v>
       </c>
@@ -3379,8 +3568,11 @@
       </c>
       <c r="I45" s="21"/>
       <c r="J45" s="24"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AJ45" s="9"/>
+      <c r="AK45" s="9"/>
+      <c r="AL45" s="9"/>
+    </row>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A46" s="25"/>
       <c r="B46" s="22" t="s">
         <v>32</v>
@@ -3408,8 +3600,20 @@
       </c>
       <c r="I46" s="22"/>
       <c r="J46" s="24"/>
-    </row>
-    <row r="47" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="AJ46" s="32">
+        <f>(($E75*V10)+($E76*36))/(V16+V10)</f>
+        <v>202703.26072073291</v>
+      </c>
+      <c r="AK46" s="32">
+        <f t="shared" ref="AK46:AL46" si="38">(($E75*W10)+($E76*36))/(W16+W10)</f>
+        <v>810813.04288293165</v>
+      </c>
+      <c r="AL46" s="32">
+        <f t="shared" si="38"/>
+        <v>1418922.8250451302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:43" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="29"/>
       <c r="B47" s="25"/>
       <c r="C47" s="25">
@@ -3437,7 +3641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>52</v>
       </c>
@@ -3469,8 +3673,14 @@
       <c r="I48" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ48" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="21" t="s">
         <v>49</v>
@@ -3479,22 +3689,22 @@
         <v>2.48</v>
       </c>
       <c r="D49" s="26">
-        <f t="shared" ref="D49:D56" si="35">$D$20</f>
+        <f t="shared" ref="D49:D56" si="39">$D$20</f>
         <v>4.7149999999999999</v>
       </c>
       <c r="E49" s="34">
-        <f t="shared" ref="E49:E56" si="36">$H$46</f>
+        <f t="shared" ref="E49:E56" si="40">$H$46</f>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F49" s="35">
-        <f t="shared" ref="F49:F56" si="37">(D49-C49)*E49*4000</f>
+        <f t="shared" ref="F49:F56" si="41">(D49-C49)*E49*4000</f>
         <v>200.56831441048033</v>
       </c>
       <c r="G49" s="36">
         <v>100</v>
       </c>
       <c r="H49" s="37">
-        <f t="shared" ref="H49:H56" si="38">F49*G49</f>
+        <f t="shared" ref="H49:H56" si="42">F49*G49</f>
         <v>20056.831441048034</v>
       </c>
       <c r="I49" s="40">
@@ -3505,8 +3715,32 @@
         <f>STDEV(H48:H56)/SQRT(9)</f>
         <v>1222.4491632804952</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AI49" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN49" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO49" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP49" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
       <c r="B50" s="21" t="s">
         <v>49</v>
@@ -3515,29 +3749,41 @@
         <v>2.52</v>
       </c>
       <c r="D50" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E50" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F50" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>196.97872489082965</v>
       </c>
       <c r="G50" s="36">
         <v>100</v>
       </c>
       <c r="H50" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>19697.872489082965</v>
       </c>
       <c r="I50" s="38" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AJ50" s="32">
+        <f>(($G73*V4)+($G76*36))/(V14+V4)</f>
+        <v>102160.56248817024</v>
+      </c>
+      <c r="AK50" s="32">
+        <f t="shared" ref="AK50:AL50" si="43">(($G73*W4)+($G76*36))/(W14+W4)</f>
+        <v>105642.24995268096</v>
+      </c>
+      <c r="AL50" s="32">
+        <f t="shared" si="43"/>
+        <v>109123.93741719166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="21" t="s">
         <v>50</v>
       </c>
@@ -3545,22 +3791,22 @@
         <v>3.11</v>
       </c>
       <c r="D51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E51" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F51" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>144.03227947598251</v>
       </c>
       <c r="G51" s="36">
         <v>100</v>
       </c>
       <c r="H51" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>14403.22794759825</v>
       </c>
       <c r="I51" s="40">
@@ -3571,8 +3817,11 @@
         <f>J49/1000</f>
         <v>1.2224491632804952</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="AJ51" s="9"/>
+      <c r="AK51" s="9"/>
+      <c r="AL51" s="9"/>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A52" s="33"/>
       <c r="B52" s="21" t="s">
         <v>50</v>
@@ -3581,28 +3830,31 @@
         <v>3.07</v>
       </c>
       <c r="D52" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E52" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F52" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>147.62186899563318</v>
       </c>
       <c r="G52" s="36">
         <v>100</v>
       </c>
       <c r="H52" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>14762.186899563318</v>
       </c>
       <c r="I52" s="38"/>
       <c r="J52" s="38"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="AJ52" s="9"/>
+      <c r="AK52" s="9"/>
+      <c r="AL52" s="9"/>
+    </row>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A53" s="33"/>
       <c r="B53" s="21" t="s">
         <v>50</v>
@@ -3611,28 +3863,40 @@
         <v>3.14</v>
       </c>
       <c r="D53" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E53" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F53" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>141.34008733624449</v>
       </c>
       <c r="G53" s="36">
         <v>100</v>
       </c>
       <c r="H53" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>14134.008733624449</v>
       </c>
       <c r="I53" s="38"/>
       <c r="J53" s="38"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="AJ53" s="32">
+        <f>(($G74*V7)+($G76*36))/(V15+V7)</f>
+        <v>127335.81828256769</v>
+      </c>
+      <c r="AK53" s="32">
+        <f t="shared" ref="AK53:AL53" si="44">(($G74*W7)+($G76*36))/(W15+W7)</f>
+        <v>206343.27313027071</v>
+      </c>
+      <c r="AL53" s="32">
+        <f t="shared" si="44"/>
+        <v>285350.7279779737</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
       <c r="B54" s="21" t="s">
         <v>51</v>
       </c>
@@ -3640,28 +3904,31 @@
         <v>3.08</v>
       </c>
       <c r="D54" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E54" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F54" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>146.72447161572046</v>
       </c>
       <c r="G54" s="36">
         <v>100</v>
       </c>
       <c r="H54" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>14672.447161572047</v>
       </c>
       <c r="I54" s="38"/>
       <c r="J54" s="39"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="AJ54" s="9"/>
+      <c r="AK54" s="9"/>
+      <c r="AL54" s="9"/>
+    </row>
+    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A55" s="33"/>
       <c r="B55" s="21" t="s">
         <v>51</v>
@@ -3670,28 +3937,31 @@
         <v>3.6</v>
       </c>
       <c r="D55" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E55" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F55" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>100.05980786026197</v>
       </c>
       <c r="G55" s="36">
         <v>100</v>
       </c>
       <c r="H55" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>10005.980786026197</v>
       </c>
       <c r="I55" s="38"/>
       <c r="J55" s="38"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="AJ55" s="9"/>
+      <c r="AK55" s="9"/>
+      <c r="AL55" s="9"/>
+    </row>
+    <row r="56" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="21" t="s">
         <v>51</v>
@@ -3700,68 +3970,80 @@
         <v>3.11</v>
       </c>
       <c r="D56" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4.7149999999999999</v>
       </c>
       <c r="E56" s="34">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2.243493449781659E-2</v>
       </c>
       <c r="F56" s="35">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>144.03227947598251</v>
       </c>
       <c r="G56" s="36">
         <v>100</v>
       </c>
       <c r="H56" s="37">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>14403.22794759825</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="AJ56" s="32">
+        <f>(($G75*V10)+($G76*36))/(V16+V10)</f>
+        <v>153494.06607165473</v>
+      </c>
+      <c r="AK56" s="32">
+        <f t="shared" ref="AK56:AL56" si="45">(($G75*W10)+($G76*36))/(W16+W10)</f>
+        <v>310976.26428661891</v>
+      </c>
+      <c r="AL56" s="32">
+        <f t="shared" si="45"/>
+        <v>468458.46250158298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="21"/>
       <c r="D57" s="26"/>
       <c r="E57" s="34"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="21"/>
       <c r="D58" s="26"/>
       <c r="E58" s="34"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="21"/>
       <c r="D59" s="26"/>
       <c r="E59" s="34"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="21"/>
       <c r="D60" s="26"/>
       <c r="E60" s="34"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="21"/>
       <c r="D61" s="26"/>
       <c r="E61" s="34"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="21"/>
       <c r="D62" s="26"/>
       <c r="E62" s="34"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="21"/>
       <c r="D63" s="26"/>
       <c r="E63" s="34"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="21"/>
       <c r="D64" s="26"/>
@@ -3800,7 +4082,7 @@
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -4044,10 +4326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D22D8F-8AAC-DB40-8C36-6BA9CEC30C6C}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4059,94 +4341,58 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M3" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4">
-        <v>37</v>
-      </c>
-      <c r="C4">
-        <v>0.5</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>370</v>
-      </c>
-      <c r="F4">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>159008.08973010862</v>
-      </c>
-      <c r="I4">
-        <v>5.9410926826545722</v>
-      </c>
-      <c r="J4">
-        <v>3.5526788019052518</v>
-      </c>
-      <c r="K4">
-        <v>8704000</v>
-      </c>
-      <c r="L4">
-        <v>4786000</v>
-      </c>
-      <c r="M4">
-        <v>488400</v>
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>37</v>
@@ -4157,37 +4403,37 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>1900</v>
+      <c r="E5" s="26">
+        <v>2004.6024450227544</v>
       </c>
       <c r="F5">
-        <v>6.28</v>
+        <v>7.97</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>28465.289008685235</v>
+      <c r="H5" t="s">
+        <v>85</v>
       </c>
       <c r="I5">
-        <v>5.9974103730460344</v>
+        <v>5.9410926826545722</v>
       </c>
       <c r="J5">
         <v>3.5526788019052518</v>
       </c>
       <c r="K5">
-        <v>9080000</v>
+        <v>49931.772002135534</v>
       </c>
       <c r="L5">
-        <v>7670000</v>
+        <v>40675.662768667476</v>
       </c>
       <c r="M5">
-        <v>1986300</v>
+        <v>102160.56248817024</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
-        <v>68</v>
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -4199,77 +4445,71 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1200</v>
+        <v>2102.4530195267785</v>
       </c>
       <c r="F6">
-        <v>6.72</v>
+        <v>7.97</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>15953.731198447349</v>
-      </c>
       <c r="I6">
-        <v>5.9578663803430603</v>
+        <v>5.9974103730460344</v>
       </c>
       <c r="J6">
         <v>3.5526788019052518</v>
       </c>
       <c r="K6">
-        <v>3990000</v>
+        <v>469642.67471635767</v>
       </c>
       <c r="L6">
-        <v>3270000.0000000005</v>
+        <v>258073.76392376923</v>
       </c>
       <c r="M6">
-        <v>93300</v>
+        <v>127335.81828256769</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>66</v>
+      <c r="A7" s="42" t="s">
+        <v>68</v>
       </c>
       <c r="B7">
         <v>37</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>370</v>
+        <v>2031.713678339619</v>
       </c>
       <c r="F7">
-        <v>4.9000000000000004</v>
+        <v>7.97</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>159008.08973010862</v>
-      </c>
       <c r="I7">
-        <v>7.0423205412648473</v>
+        <v>5.9578663803430603</v>
       </c>
       <c r="J7">
-        <v>4.6026788019052516</v>
+        <v>3.5526788019052518</v>
       </c>
       <c r="K7">
-        <v>8704000</v>
+        <v>240266.83276978548</v>
       </c>
       <c r="L7">
-        <v>4786000</v>
+        <v>202703.26072073291</v>
       </c>
       <c r="M7">
-        <v>488400</v>
+        <v>153494.06607165473</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>37</v>
@@ -4280,37 +4520,34 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8">
-        <v>1900</v>
+      <c r="E8" s="34">
+        <v>2018.4097800910176</v>
       </c>
       <c r="F8">
-        <v>6.28</v>
+        <v>7.97</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>28465.289008685235</v>
-      </c>
       <c r="I8">
-        <v>7.3191562857132659</v>
+        <v>7.0423205412648473</v>
       </c>
       <c r="J8">
         <v>4.6026788019052516</v>
       </c>
       <c r="K8">
-        <v>9080000</v>
+        <v>198827.08800854211</v>
       </c>
       <c r="L8">
-        <v>7670000</v>
+        <v>162702.65107466988</v>
       </c>
       <c r="M8">
-        <v>1986300</v>
+        <v>105642.24995268096</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
-        <v>68</v>
+      <c r="A9" t="s">
+        <v>67</v>
       </c>
       <c r="B9">
         <v>37</v>
@@ -4322,77 +4559,71 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1200</v>
+        <v>2409.8120781071138</v>
       </c>
       <c r="F9">
-        <v>6.72</v>
+        <v>7.97</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>15953.731198447349</v>
-      </c>
       <c r="I9">
-        <v>7.1230974093355544</v>
+        <v>7.3191562857132659</v>
       </c>
       <c r="J9">
         <v>4.6026788019052516</v>
       </c>
       <c r="K9">
-        <v>3990000</v>
+        <v>1877670.6988654307</v>
       </c>
       <c r="L9">
-        <v>3270000.0000000005</v>
+        <v>1032295.0556950769</v>
       </c>
       <c r="M9">
-        <v>93300</v>
+        <v>206343.27313027071</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>66</v>
+      <c r="A10" s="42" t="s">
+        <v>68</v>
       </c>
       <c r="B10">
         <v>37</v>
       </c>
-      <c r="C10" s="42">
-        <v>3.5</v>
+      <c r="C10">
+        <v>2</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>370</v>
+        <v>2126.8547133584771</v>
       </c>
       <c r="F10">
-        <v>4.9000000000000004</v>
+        <v>7.97</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>159008.08973010862</v>
-      </c>
-      <c r="I10" s="32">
-        <v>8.1590256539532806</v>
+      <c r="I10">
+        <v>7.1230974093355544</v>
       </c>
       <c r="J10">
-        <v>5.6526788019052514</v>
+        <v>4.6026788019052516</v>
       </c>
       <c r="K10">
-        <v>8704000</v>
+        <v>960167.33107914194</v>
       </c>
       <c r="L10">
-        <v>4786000</v>
+        <v>810813.04288293165</v>
       </c>
       <c r="M10">
-        <v>488400</v>
+        <v>310976.26428661891</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11">
         <v>37</v>
@@ -4403,37 +4634,34 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11">
-        <v>1900</v>
+      <c r="E11" s="35">
+        <v>2032.2171151592811</v>
       </c>
       <c r="F11">
-        <v>6.28</v>
+        <v>7.97</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>28465.289008685235</v>
-      </c>
       <c r="I11" s="32">
-        <v>8.7417149861139336</v>
+        <v>8.1590256539532806</v>
       </c>
       <c r="J11">
         <v>5.6526788019052514</v>
       </c>
       <c r="K11">
-        <v>9080000</v>
+        <v>347722.40401494864</v>
       </c>
       <c r="L11">
-        <v>7670000</v>
+        <v>284729.63938067225</v>
       </c>
       <c r="M11">
-        <v>1986300</v>
+        <v>109123.93741719166</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
-        <v>68</v>
+      <c r="A12" t="s">
+        <v>67</v>
       </c>
       <c r="B12">
         <v>37</v>
@@ -4445,31 +4673,66 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1200</v>
+        <v>2717.1711366874492</v>
       </c>
       <c r="F12">
-        <v>6.72</v>
+        <v>7.97</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <v>15953.731198447349</v>
-      </c>
       <c r="I12" s="32">
-        <v>8.3254063150872923</v>
+        <v>8.7417149861139336</v>
       </c>
       <c r="J12">
         <v>5.6526788019052514</v>
       </c>
       <c r="K12">
-        <v>3990000</v>
+        <v>3285698.7230145033</v>
       </c>
       <c r="L12">
-        <v>3270000.0000000005</v>
+        <v>1806516.3474663845</v>
       </c>
       <c r="M12">
-        <v>93300</v>
+        <v>285350.7279779737</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13">
+        <v>37</v>
+      </c>
+      <c r="C13" s="42">
+        <v>3.5</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2221.9957483773346</v>
+      </c>
+      <c r="F13">
+        <v>7.97</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="32">
+        <v>8.3254063150872923</v>
+      </c>
+      <c r="J13">
+        <v>5.6526788019052514</v>
+      </c>
+      <c r="K13">
+        <v>1680067.8293884983</v>
+      </c>
+      <c r="L13">
+        <v>1418922.8250451302</v>
+      </c>
+      <c r="M13">
+        <v>468458.46250158298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>